<commit_message>
A130.xlsx covers everything in WD schema
</commit_message>
<xml_diff>
--- a/painting/painting_template.xlsx
+++ b/painting/painting_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tbaker/github/dcmi/dcap/painting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A117473C-FB95-F142-9C43-5054C993A95B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6604A38-5EDF-C54A-893E-2A4BDA87D26D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12320" yWindow="-28340" windowWidth="50800" windowHeight="27260" xr2:uid="{07BF049F-611D-AA48-83C2-8A2FFB416598}"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>Value entity ID</t>
   </si>
   <si>
-    <t>Value list</t>
-  </si>
-  <si>
     <t>Value URI stem</t>
   </si>
   <si>
@@ -82,6 +79,9 @@
   </si>
   <si>
     <t>Max</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -117,13 +117,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -442,7 +445,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="259" zoomScaleNormal="259" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -454,10 +457,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="3"/>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
@@ -472,6 +475,8 @@
       <c r="L1" s="2"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
@@ -485,7 +490,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L2" s="2"/>
     </row>
@@ -509,31 +514,31 @@
         <v>9</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="K3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:J2"/>
     <mergeCell ref="K2:L2"/>
+    <mergeCell ref="A1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>